<commit_message>
This is my new code for marketing...
</commit_message>
<xml_diff>
--- a/Externaldata/Cams_login.xlsx
+++ b/Externaldata/Cams_login.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nirak\Desktop\Radhakrushna_OASYS\Cams_Oasys\Externaldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA1BCFF-DF79-4038-B7DE-FE8E5F780BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F9D815-E812-4B5E-BF90-5A7C7819E4F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1C652985-6E6C-4A4D-8ADE-F8717E9CC80D}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -127,7 +127,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -516,25 +515,25 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.33203125"/>
-    <col min="2" max="2" customWidth="true" width="13.77734375"/>
-    <col min="3" max="3" customWidth="true" width="13.88671875"/>
-    <col min="4" max="4" customWidth="true" width="24.21875"/>
-    <col min="5" max="5" customWidth="true" width="21.33203125"/>
-    <col min="6" max="6" customWidth="true" width="13.6640625"/>
-    <col min="7" max="7" customWidth="true" width="15.109375"/>
-    <col min="8" max="8" customWidth="true" width="19.77734375"/>
-    <col min="9" max="9" customWidth="true" width="15.21875"/>
-    <col min="10" max="10" customWidth="true" width="16.0"/>
-    <col min="11" max="11" customWidth="true" width="17.77734375"/>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+    <col min="4" max="4" width="24.21875" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" customWidth="1"/>
+    <col min="8" max="8" width="19.77734375" customWidth="1"/>
+    <col min="9" max="9" width="15.21875" customWidth="1"/>
+    <col min="10" max="10" width="16" customWidth="1"/>
+    <col min="11" max="11" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1">
+    <row r="1" spans="1:12" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -572,11 +571,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C2" t="s">
@@ -607,7 +606,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -642,7 +641,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -683,6 +682,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{6146078E-71CB-4BC2-A777-5D812A73054E}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{442AE6D5-05F5-4AA0-AD31-06A023A076F0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>